<commit_message>
Updated project plan 4/13
</commit_message>
<xml_diff>
--- a/misc_files/project_plan.xlsx
+++ b/misc_files/project_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPSC224_01_Group6\misc_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46AB839-9EE0-449A-A821-B9F82E5DE7F9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC5FCAE-2EFA-4BE9-B44A-A95065B3FAD2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -108,15 +108,6 @@
   </si>
   <si>
     <t>Create Hand.java</t>
-  </si>
-  <si>
-    <t>Create BuildPhase.java</t>
-  </si>
-  <si>
-    <t>Create SpacePhase.java</t>
-  </si>
-  <si>
-    <t>Create Scorecard.java</t>
   </si>
   <si>
     <t>Create source code based off current UML spec</t>
@@ -958,7 +949,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,7 +983,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="2"/>
@@ -1012,8 +1003,12 @@
         <v>43203</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="2">
+        <v>43203</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1029,12 +1024,16 @@
         <v>43203</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="2">
+        <v>43203</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1053,9 +1052,15 @@
       <c r="D6" s="2">
         <v>43203</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="E6" s="1">
+        <v>100</v>
+      </c>
+      <c r="F6" s="2">
+        <v>43202</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1070,13 +1075,19 @@
       <c r="D7" s="2">
         <v>43203</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="1">
+        <v>100</v>
+      </c>
+      <c r="F7" s="2">
+        <v>43202</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1090,14 +1101,18 @@
         <v>15</v>
       </c>
       <c r="C9" s="1">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="D9" s="2">
         <v>43221</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="E9" s="1">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1107,62 +1122,42 @@
         <v>15</v>
       </c>
       <c r="C10" s="1">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="D10" s="2">
         <v>43221</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="E10" s="1">
+        <v>95</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
-        <v>43221</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2">
-        <v>43221</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>43221</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1205,10 +1200,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
@@ -1233,15 +1238,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1426,6 +1422,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B616F827-B535-4D73-8E2B-1E3703C34EC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1438,14 +1442,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed a bug in readScore
</commit_message>
<xml_diff>
--- a/misc_files/project_plan.xlsx
+++ b/misc_files/project_plan.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPSC224_01_Group6\misc_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC5FCAE-2EFA-4BE9-B44A-A95065B3FAD2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80B453A-0862-44BD-87BC-14210C26F7B9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WeekMar25" sheetId="1" r:id="rId1"/>
     <sheet name="WeekApr1" sheetId="2" r:id="rId2"/>
     <sheet name="WeekApr8" sheetId="3" r:id="rId3"/>
+    <sheet name="WeekApr15" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -117,6 +118,18 @@
   </si>
   <si>
     <t>Create a test plan document</t>
+  </si>
+  <si>
+    <t>Work on coding the game</t>
+  </si>
+  <si>
+    <t>Work on build phase</t>
+  </si>
+  <si>
+    <t>Work on space phase</t>
+  </si>
+  <si>
+    <t>Work on scorecard</t>
   </si>
 </sst>
 </file>
@@ -146,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -169,11 +182,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -184,6 +208,8 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -948,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E23D512-EF74-419A-80CC-6C1FE1BF1CBE}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,43 +1230,223 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CB9F3D-F05C-4B74-A90E-4F5478C2A8FE}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43221</v>
+      </c>
+      <c r="E3" s="1">
+        <v>90</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43221</v>
+      </c>
+      <c r="E4" s="1">
+        <v>90</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3.75</v>
+      </c>
+      <c r="D5" s="7">
+        <v>43221</v>
+      </c>
+      <c r="E5" s="1">
+        <v>90</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
-      <Value>Group Project</Value>
-    </Doc_x0020_Type>
-    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
-      <UserInfo>
-        <DisplayName>Greenside, Trevor Michael</DisplayName>
-        <AccountId>146</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
-        <AccountId>609</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Hartwell, Harvey C</DisplayName>
-        <AccountId>606</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC2685C84B160940930467983553E2DA" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64476ae877ed79da2175079bb3e4829a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9b0d329a-e114-4ba8-bee9-62c1c786fd9a" xmlns:ns3="013b2221-5078-4f34-9921-a0ecb049492d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="564df3335efcf36b4d09ae51e046af81" ns2:_="" ns3:_="">
     <xsd:import namespace="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
@@ -1421,10 +1627,57 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Type xmlns="9b0d329a-e114-4ba8-bee9-62c1c786fd9a">
+      <Value>Group Project</Value>
+    </Doc_x0020_Type>
+    <SharedWithUsers xmlns="013b2221-5078-4f34-9921-a0ecb049492d">
+      <UserInfo>
+        <DisplayName>Greenside, Trevor Michael</DisplayName>
+        <AccountId>146</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kopczynski, Scott Patrick</DisplayName>
+        <AccountId>609</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Hartwell, Harvey C</DisplayName>
+        <AccountId>606</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{309F765C-3428-4D4C-A6F6-5C1534E87CBC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
+    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1447,20 +1700,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{309F765C-3428-4D4C-A6F6-5C1534E87CBC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{977C615D-C0CF-4E54-82E4-40DCE513F318}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9b0d329a-e114-4ba8-bee9-62c1c786fd9a"/>
-    <ds:schemaRef ds:uri="013b2221-5078-4f34-9921-a0ecb049492d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>